<commit_message>
DSA Binary Search Answers Practice
</commit_message>
<xml_diff>
--- a/00_QnA/00_DSA Questions.xlsx
+++ b/00_QnA/00_DSA Questions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="123">
   <si>
     <t>S. No</t>
   </si>
@@ -384,13 +384,25 @@
   </si>
   <si>
     <t>https://www.naukri.com/code360/problems/square-root-integral_893351</t>
+  </si>
+  <si>
+    <t>1011. Capacity To Ship Packages Within D Days</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/capacity-to-ship-packages-within-d-days/description/</t>
+  </si>
+  <si>
+    <t>1283. Find the Smallest Divisor Given a Threshold</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-the-smallest-divisor-given-a-threshold/description/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,6 +443,14 @@
     <font>
       <sz val="8"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -484,7 +504,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -500,6 +520,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -747,10 +770,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1695,13 +1718,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="2" topLeftCell="I33" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="8" ySplit="2" topLeftCell="I9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B53" sqref="B53"/>
+      <selection pane="bottomRight" activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,6 +1744,10 @@
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
+      <c r="H1" s="10">
+        <f>SUM(H3:H5)</f>
+        <v>47</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1770,7 +1797,7 @@
       </c>
       <c r="H3" s="6">
         <f>COUNTIF($D:$D,$G3)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1797,7 +1824,7 @@
       </c>
       <c r="H4" s="6">
         <f>COUNTIF($D:$D,$G4)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2498,7 +2525,7 @@
         <v>44</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>86</v>
@@ -2518,7 +2545,7 @@
         <v>44</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>87</v>
@@ -2804,6 +2831,46 @@
         <v>116</v>
       </c>
       <c r="F54" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>53</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>54</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F56" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2857,9 +2924,11 @@
     <hyperlink ref="E54" r:id="rId43"/>
     <hyperlink ref="E53" r:id="rId44"/>
     <hyperlink ref="E51" r:id="rId45"/>
+    <hyperlink ref="E56" r:id="rId46"/>
+    <hyperlink ref="E55" r:id="rId47"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId46"/>
-  <drawing r:id="rId47"/>
+  <pageSetup orientation="portrait" r:id="rId48"/>
+  <drawing r:id="rId49"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DSA Linked List Practice
</commit_message>
<xml_diff>
--- a/00_QnA/00_DSA Questions.xlsx
+++ b/00_QnA/00_DSA Questions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="161">
   <si>
     <t>S. No</t>
   </si>
@@ -468,6 +468,48 @@
   </si>
   <si>
     <t>141. Linked List Cycle</t>
+  </si>
+  <si>
+    <t>234. Palindrome Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/palindrome-linked-list/description/</t>
+  </si>
+  <si>
+    <t>328. Odd Even Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/odd-even-linked-list/description/</t>
+  </si>
+  <si>
+    <t>2095. Delete the Middle Node of a Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/delete-the-middle-node-of-a-linked-list/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-nth-node-from-end-of-list/description/</t>
+  </si>
+  <si>
+    <t>19. Remove Nth Node From End of List</t>
+  </si>
+  <si>
+    <t>148. Sort List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sort-list/</t>
+  </si>
+  <si>
+    <t>Find length of Loop</t>
+  </si>
+  <si>
+    <t>https://www.naukri.com/code360/problems/find-length-of-loop_8160455</t>
+  </si>
+  <si>
+    <t>142. Linked List Cycle II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/linked-list-cycle-ii/description/</t>
   </si>
 </sst>
 </file>
@@ -842,10 +884,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1790,13 +1832,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="8" ySplit="2" topLeftCell="I48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="2" topLeftCell="I45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D66" sqref="D66"/>
+      <selection pane="bottomRight" activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1818,7 +1860,7 @@
       <c r="E1" s="10"/>
       <c r="H1" s="9">
         <f>SUM(H3:H5)</f>
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1869,7 +1911,7 @@
       </c>
       <c r="H3" s="6">
         <f>COUNTIF($D:$D,$G3)</f>
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1896,7 +1938,7 @@
       </c>
       <c r="H4" s="6">
         <f>COUNTIF($D:$D,$G4)</f>
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3183,6 +3225,146 @@
         <v>144</v>
       </c>
       <c r="F68" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>67</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>68</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>69</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>70</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>71</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F73" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>72</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F74" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>73</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F75" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3250,9 +3432,16 @@
     <hyperlink ref="E66" r:id="rId57"/>
     <hyperlink ref="E68" r:id="rId58"/>
     <hyperlink ref="E67" r:id="rId59"/>
+    <hyperlink ref="E71" r:id="rId60"/>
+    <hyperlink ref="E72" r:id="rId61"/>
+    <hyperlink ref="E74" r:id="rId62"/>
+    <hyperlink ref="E73" r:id="rId63"/>
+    <hyperlink ref="E75" r:id="rId64"/>
+    <hyperlink ref="E70" r:id="rId65"/>
+    <hyperlink ref="E69" r:id="rId66"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId60"/>
-  <drawing r:id="rId61"/>
+  <pageSetup orientation="portrait" r:id="rId67"/>
+  <drawing r:id="rId68"/>
 </worksheet>
 </file>
</xml_diff>